<commit_message>
Finalization of all WASABI N-of-Many tasks
</commit_message>
<xml_diff>
--- a/fMRI Tasks/N-Of-Many/WASABI distractmap/nbackorder/N-back-0_1.xlsx
+++ b/fMRI Tasks/N-Of-Many/WASABI distractmap/nbackorder/N-back-0_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\canlab\WASABI_public\fMRI Tasks\N-Of-Many\WASABI distractmap\nbackorder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\canlab\WASABI_public\fMRI Tasks\N-Of-Many\WASABI distractmap\nbackorder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DABC234-6834-4376-A92B-55A9953911E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BCF083-DA8B-4F04-9A70-90BDFF19E137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-24120" windowWidth="38640" windowHeight="23025" xr2:uid="{F2F223E6-6D4D-474F-AA9E-867F0F7D577D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="24312" xr2:uid="{F2F223E6-6D4D-474F-AA9E-867F0F7D577D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>square</t>
   </si>
@@ -50,12 +50,6 @@
   </si>
   <si>
     <t>[0, 0]</t>
-  </si>
-  <si>
-    <t>[-0.2, 0.2]</t>
-  </si>
-  <si>
-    <t>[-0.2, -0.2]</t>
   </si>
 </sst>
 </file>
@@ -513,15 +507,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828E0459-BD4B-48E0-8970-09453A3EFA33}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
       </c>
@@ -544,7 +538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>7</v>
       </c>
@@ -556,7 +550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7</v>
       </c>
@@ -568,7 +562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -580,7 +574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>8</v>
       </c>
@@ -592,7 +586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -604,7 +598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -616,7 +610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
@@ -624,28 +618,6 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11">
         <v>1</v>
       </c>
     </row>

</xml_diff>